<commit_message>
atualizei o grafico de gantt
</commit_message>
<xml_diff>
--- a/Documentação/Date tracking Gantt chart1.xlsx
+++ b/Documentação/Date tracking Gantt chart1.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{238E645D-5ADF-4AAF-A7B8-921C2C5DE908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E30BBE-F719-4DB1-AB81-838C4AFF6D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1166,9 +1166,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="10" fillId="11" borderId="17" xfId="11" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1176,6 +1173,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="10" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2248,8 +2248,8 @@
   </sheetPr>
   <dimension ref="A1:BK33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="C5" s="56">
         <f ca="1">IFERROR(IF(MIN(Milestones34[Start])=0,TODAY(),MIN(Milestones34[Start])),TODAY())</f>
-        <v>44623</v>
+        <v>44629</v>
       </c>
       <c r="E5" s="73"/>
       <c r="H5" s="36"/>
@@ -2425,14 +2425,14 @@
       <c r="K5" s="37"/>
       <c r="L5" s="37"/>
       <c r="M5" s="38"/>
-      <c r="O5" s="119" t="s">
+      <c r="O5" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="119"/>
-      <c r="Q5" s="119"/>
-      <c r="R5" s="119"/>
-      <c r="S5" s="119"/>
-      <c r="T5" s="119"/>
+      <c r="P5" s="122"/>
+      <c r="Q5" s="122"/>
+      <c r="R5" s="122"/>
+      <c r="S5" s="122"/>
+      <c r="T5" s="122"/>
       <c r="U5" s="57">
         <v>0</v>
       </c>
@@ -2525,139 +2525,139 @@
       <c r="G7" s="23"/>
       <c r="H7" s="109">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>44623</v>
+        <v>44629</v>
       </c>
       <c r="I7" s="110">
         <f ca="1">H7+1</f>
-        <v>44624</v>
+        <v>44630</v>
       </c>
       <c r="J7" s="110">
         <f t="shared" ref="J7:AB7" ca="1" si="0">I7+1</f>
-        <v>44625</v>
+        <v>44631</v>
       </c>
       <c r="K7" s="110">
         <f ca="1">J7+1</f>
-        <v>44626</v>
+        <v>44632</v>
       </c>
       <c r="L7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44627</v>
+        <v>44633</v>
       </c>
       <c r="M7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44628</v>
+        <v>44634</v>
       </c>
       <c r="N7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44629</v>
+        <v>44635</v>
       </c>
       <c r="O7" s="110">
         <f ca="1">N7+1</f>
-        <v>44630</v>
+        <v>44636</v>
       </c>
       <c r="P7" s="110">
         <f ca="1">O7+1</f>
-        <v>44631</v>
+        <v>44637</v>
       </c>
       <c r="Q7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44632</v>
+        <v>44638</v>
       </c>
       <c r="R7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44633</v>
+        <v>44639</v>
       </c>
       <c r="S7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44634</v>
+        <v>44640</v>
       </c>
       <c r="T7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44635</v>
+        <v>44641</v>
       </c>
       <c r="U7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44636</v>
+        <v>44642</v>
       </c>
       <c r="V7" s="110">
         <f ca="1">U7+1</f>
-        <v>44637</v>
+        <v>44643</v>
       </c>
       <c r="W7" s="110">
         <f ca="1">V7+1</f>
-        <v>44638</v>
+        <v>44644</v>
       </c>
       <c r="X7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44639</v>
+        <v>44645</v>
       </c>
       <c r="Y7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44640</v>
+        <v>44646</v>
       </c>
       <c r="Z7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44641</v>
+        <v>44647</v>
       </c>
       <c r="AA7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44642</v>
+        <v>44648</v>
       </c>
       <c r="AB7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44643</v>
+        <v>44649</v>
       </c>
       <c r="AC7" s="110">
         <f ca="1">AB7+1</f>
-        <v>44644</v>
-      </c>
-      <c r="AD7" s="120">
+        <v>44650</v>
+      </c>
+      <c r="AD7" s="119">
         <f ca="1">AC7+1</f>
-        <v>44645</v>
+        <v>44651</v>
       </c>
       <c r="AE7" s="110">
         <f t="shared" ref="AE7" ca="1" si="1">AD7+1</f>
-        <v>44646</v>
+        <v>44652</v>
       </c>
       <c r="AF7" s="110">
         <f t="shared" ref="AF7" ca="1" si="2">AE7+1</f>
-        <v>44647</v>
+        <v>44653</v>
       </c>
       <c r="AG7" s="110">
         <f t="shared" ref="AG7" ca="1" si="3">AF7+1</f>
-        <v>44648</v>
+        <v>44654</v>
       </c>
       <c r="AH7" s="110">
         <f t="shared" ref="AH7" ca="1" si="4">AG7+1</f>
-        <v>44649</v>
+        <v>44655</v>
       </c>
       <c r="AI7" s="110">
         <f t="shared" ref="AI7" ca="1" si="5">AH7+1</f>
-        <v>44650</v>
+        <v>44656</v>
       </c>
       <c r="AJ7" s="110">
         <f ca="1">AI7+1</f>
-        <v>44651</v>
+        <v>44657</v>
       </c>
       <c r="AK7" s="110">
         <f ca="1">AJ7+1</f>
-        <v>44652</v>
+        <v>44658</v>
       </c>
       <c r="AL7" s="110">
         <f ca="1">AK7+1</f>
-        <v>44653</v>
+        <v>44659</v>
       </c>
       <c r="AM7" s="110">
         <f ca="1">AL7+1</f>
-        <v>44654</v>
+        <v>44660</v>
       </c>
       <c r="AN7" s="110">
         <f t="shared" ref="AN7" ca="1" si="6">AM7+1</f>
-        <v>44655</v>
+        <v>44661</v>
       </c>
       <c r="AO7" s="110">
         <f t="shared" ref="AO7" ca="1" si="7">AN7+1</f>
-        <v>44656</v>
+        <v>44662</v>
       </c>
       <c r="AP7" s="110"/>
       <c r="AQ7" s="110"/>
@@ -2706,7 +2706,7 @@
       </c>
       <c r="I8" s="107" t="str">
         <f ca="1">LEFT(TEXT(I7,"ddd"),1)</f>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="J8" s="107" t="str">
         <f ca="1">LEFT(TEXT(J7,"ddd"),1)</f>
@@ -2714,19 +2714,19 @@
       </c>
       <c r="K8" s="107" t="str">
         <f t="shared" ref="K8:AC8" ca="1" si="8">LEFT(TEXT(K7,"ddd"),1)</f>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="L8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="M8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="N8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="O8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -2734,7 +2734,7 @@
       </c>
       <c r="P8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="Q8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -2742,19 +2742,19 @@
       </c>
       <c r="R8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="S8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="T8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="U8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="V8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -2762,7 +2762,7 @@
       </c>
       <c r="W8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="X8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -2770,27 +2770,27 @@
       </c>
       <c r="Y8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="Z8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AA8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AB8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="AC8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
         <v>q</v>
       </c>
-      <c r="AD8" s="121" t="str">
+      <c r="AD8" s="120" t="str">
         <f t="shared" ref="AD8:AJ8" ca="1" si="9">LEFT(TEXT(AD7,"ddd"),1)</f>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AE8" s="107" t="str">
         <f t="shared" ca="1" si="9"/>
@@ -2798,19 +2798,19 @@
       </c>
       <c r="AF8" s="107" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="AG8" s="107" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AH8" s="107" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AI8" s="107" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="AJ8" s="107" t="str">
         <f t="shared" ca="1" si="9"/>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="AK8" s="107" t="str">
         <f t="shared" ref="AK8:AL8" ca="1" si="10">LEFT(TEXT(AK7,"ddd"),1)</f>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AL8" s="107" t="str">
         <f t="shared" ca="1" si="10"/>
@@ -2826,15 +2826,15 @@
       </c>
       <c r="AM8" s="107" t="str">
         <f t="shared" ref="AM8:AO8" ca="1" si="11">LEFT(TEXT(AM7,"ddd"),1)</f>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="AN8" s="107" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AO8" s="107" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AP8" s="107"/>
       <c r="AQ8" s="107"/>
@@ -3101,11 +3101,11 @@
         <v>1</v>
       </c>
       <c r="E11" s="51">
-        <f ca="1">TODAY()-33</f>
-        <v>44623</v>
+        <f ca="1">TODAY()-40</f>
+        <v>44629</v>
       </c>
       <c r="F11" s="49">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="G11" s="117"/>
       <c r="H11" s="118" t="str">
@@ -3277,10 +3277,10 @@
         <v>1</v>
       </c>
       <c r="E12" s="51">
-        <f ca="1">TODAY()-23</f>
-        <v>44633</v>
-      </c>
-      <c r="F12" s="122">
+        <f ca="1">TODAY()-30</f>
+        <v>44639</v>
+      </c>
+      <c r="F12" s="121">
         <v>15</v>
       </c>
       <c r="G12" s="117"/>
@@ -3450,11 +3450,11 @@
         <v>1</v>
       </c>
       <c r="E13" s="51">
-        <f ca="1">TODAY()-25</f>
-        <v>44631</v>
+        <f ca="1">TODAY()-32</f>
+        <v>44637</v>
       </c>
       <c r="F13" s="49">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G13" s="117"/>
       <c r="H13" s="118" t="str">
@@ -3626,11 +3626,11 @@
         <v>1</v>
       </c>
       <c r="E14" s="51">
-        <f ca="1">TODAY()-12</f>
-        <v>44644</v>
+        <f ca="1">TODAY()-19</f>
+        <v>44650</v>
       </c>
       <c r="F14" s="49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G14" s="117"/>
       <c r="H14" s="118" t="str">
@@ -3799,8 +3799,8 @@
         <v>1</v>
       </c>
       <c r="E15" s="51">
-        <f ca="1">TODAY()-21</f>
-        <v>44635</v>
+        <f ca="1">TODAY()-28</f>
+        <v>44641</v>
       </c>
       <c r="F15" s="49">
         <v>9</v>
@@ -4144,8 +4144,8 @@
         <v>1</v>
       </c>
       <c r="E17" s="51">
-        <f ca="1">TODAY()-26</f>
-        <v>44630</v>
+        <f ca="1">TODAY()-32</f>
+        <v>44637</v>
       </c>
       <c r="F17" s="49">
         <v>13</v>
@@ -4320,8 +4320,8 @@
         <v>1</v>
       </c>
       <c r="E18" s="51">
-        <f ca="1">TODAY()-22</f>
-        <v>44634</v>
+        <f ca="1">TODAY()-29</f>
+        <v>44640</v>
       </c>
       <c r="F18" s="49">
         <v>14</v>
@@ -4496,8 +4496,8 @@
         <v>1</v>
       </c>
       <c r="E19" s="51">
-        <f ca="1">TODAY()-28</f>
-        <v>44628</v>
+        <f ca="1">TODAY()-35</f>
+        <v>44634</v>
       </c>
       <c r="F19" s="49">
         <v>10</v>
@@ -4672,8 +4672,8 @@
         <v>1</v>
       </c>
       <c r="E20" s="51">
-        <f ca="1">TODAY()-18</f>
-        <v>44638</v>
+        <f ca="1">TODAY()-25</f>
+        <v>44644</v>
       </c>
       <c r="F20" s="49">
         <v>5</v>
@@ -5014,8 +5014,8 @@
         <v>1</v>
       </c>
       <c r="E22" s="51">
-        <f ca="1">TODAY()-23</f>
-        <v>44633</v>
+        <f ca="1">TODAY()-30</f>
+        <v>44639</v>
       </c>
       <c r="F22" s="49">
         <v>8</v>
@@ -5190,8 +5190,8 @@
         <v>1</v>
       </c>
       <c r="E23" s="51">
-        <f ca="1">TODAY()-18</f>
-        <v>44638</v>
+        <f ca="1">TODAY()-25</f>
+        <v>44644</v>
       </c>
       <c r="F23" s="49">
         <v>8</v>
@@ -5366,8 +5366,8 @@
         <v>1</v>
       </c>
       <c r="E24" s="51">
-        <f ca="1">TODAY()-9</f>
-        <v>44647</v>
+        <f ca="1">TODAY()-16</f>
+        <v>44653</v>
       </c>
       <c r="F24" s="49">
         <v>15</v>
@@ -5542,8 +5542,8 @@
         <v>1</v>
       </c>
       <c r="E25" s="51">
-        <f ca="1">TODAY()-21</f>
-        <v>44635</v>
+        <f ca="1">TODAY()-28</f>
+        <v>44641</v>
       </c>
       <c r="F25" s="49">
         <v>13</v>
@@ -5887,8 +5887,8 @@
         <v>1</v>
       </c>
       <c r="E27" s="51">
-        <f ca="1">TODAY()-22</f>
-        <v>44634</v>
+        <f ca="1">TODAY()-29</f>
+        <v>44640</v>
       </c>
       <c r="F27" s="49">
         <v>15</v>
@@ -6063,8 +6063,8 @@
         <v>1</v>
       </c>
       <c r="E28" s="51">
-        <f ca="1">TODAY()-27</f>
-        <v>44629</v>
+        <f ca="1">TODAY()-34</f>
+        <v>44635</v>
       </c>
       <c r="F28" s="49">
         <v>15</v>
@@ -6239,8 +6239,8 @@
         <v>1</v>
       </c>
       <c r="E29" s="51">
-        <f ca="1">TODAY()-26</f>
-        <v>44630</v>
+        <f ca="1">TODAY()-40</f>
+        <v>44629</v>
       </c>
       <c r="F29" s="49">
         <v>10</v>
@@ -6314,7 +6314,7 @@
       </c>
       <c r="E30" s="51">
         <f ca="1">TODAY()</f>
-        <v>44656</v>
+        <v>44669</v>
       </c>
       <c r="F30" s="49">
         <v>1</v>
@@ -6452,9 +6452,9 @@
         <f ca="1">IFERROR(IF(LEN(Milestones34[[#This Row],[Days]])=0,"",IF(AND(AN$7=$E30,$F30=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
-      <c r="AO30" s="32">
+      <c r="AO30" s="32" t="str">
         <f ca="1">IFERROR(IF(LEN(Milestones34[[#This Row],[Days]])=0,"",IF(AND(AO$7=$E30,$F30=1),Milestone_Marker,"")),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="AP30" s="32"/>
       <c r="AQ30" s="32"/>
@@ -6878,7 +6878,7 @@
       </c>
       <c r="C5" s="56">
         <f ca="1">IFERROR(IF(MIN(Milestones3[Start])=0,TODAY(),MIN(Milestones3[Start])),TODAY())</f>
-        <v>44653</v>
+        <v>44666</v>
       </c>
       <c r="E5" s="73"/>
       <c r="H5" s="39"/>
@@ -6887,14 +6887,14 @@
       <c r="K5" s="40"/>
       <c r="L5" s="40"/>
       <c r="M5" s="41"/>
-      <c r="O5" s="119" t="s">
+      <c r="O5" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="119"/>
-      <c r="Q5" s="119"/>
-      <c r="R5" s="119"/>
-      <c r="S5" s="119"/>
-      <c r="T5" s="119"/>
+      <c r="P5" s="122"/>
+      <c r="Q5" s="122"/>
+      <c r="R5" s="122"/>
+      <c r="S5" s="122"/>
+      <c r="T5" s="122"/>
       <c r="U5" s="57">
         <v>13</v>
       </c>
@@ -6924,7 +6924,7 @@
       <c r="N6" s="29"/>
       <c r="O6" s="29" t="str">
         <f ca="1">IF(TEXT(O7,"mmmm")=H6,"",TEXT(O7,"mmmm"))</f>
-        <v/>
+        <v>maio</v>
       </c>
       <c r="P6" s="29"/>
       <c r="Q6" s="29"/>
@@ -6944,7 +6944,7 @@
       <c r="AB6" s="29"/>
       <c r="AC6" s="29" t="str">
         <f ca="1">IF(OR(TEXT(AC7,"mmmm")=V6,TEXT(AC7,"mmmm")=O6,TEXT(AC7,"mmmm")=H6),"",TEXT(AC7,"mmmm"))</f>
-        <v>maio</v>
+        <v/>
       </c>
       <c r="AD6" s="29"/>
       <c r="AE6" s="29"/>
@@ -6964,7 +6964,7 @@
       <c r="AP6" s="29"/>
       <c r="AQ6" s="29" t="str">
         <f ca="1">IF(OR(TEXT(AQ7,"mmmm")=AJ6,TEXT(AQ7,"mmmm")=AC6,TEXT(AQ7,"mmmm")=V6,TEXT(AQ7,"mmmm")=O6),"",TEXT(AQ7,"mmmm"))</f>
-        <v/>
+        <v>junho</v>
       </c>
       <c r="AR6" s="29"/>
       <c r="AS6" s="29"/>
@@ -6984,7 +6984,7 @@
       <c r="BD6" s="29"/>
       <c r="BE6" s="29" t="str">
         <f ca="1">IF(OR(TEXT(BE7,"mmmm")=AX6,TEXT(BE7,"mmmm")=AQ6,TEXT(BE7,"mmmm")=AJ6,TEXT(BE7,"mmmm")=AC6),"",TEXT(BE7,"mmmm"))</f>
-        <v>junho</v>
+        <v/>
       </c>
       <c r="BF6" s="29"/>
       <c r="BG6" s="29"/>
@@ -6999,227 +6999,227 @@
       <c r="G7" s="23"/>
       <c r="H7" s="61">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>44666</v>
+        <v>44679</v>
       </c>
       <c r="I7" s="62">
         <f ca="1">H7+1</f>
-        <v>44667</v>
+        <v>44680</v>
       </c>
       <c r="J7" s="62">
         <f t="shared" ref="J7:AW7" ca="1" si="0">I7+1</f>
-        <v>44668</v>
+        <v>44681</v>
       </c>
       <c r="K7" s="62">
         <f ca="1">J7+1</f>
-        <v>44669</v>
+        <v>44682</v>
       </c>
       <c r="L7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44670</v>
+        <v>44683</v>
       </c>
       <c r="M7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44671</v>
+        <v>44684</v>
       </c>
       <c r="N7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44672</v>
+        <v>44685</v>
       </c>
       <c r="O7" s="62">
         <f ca="1">N7+1</f>
-        <v>44673</v>
+        <v>44686</v>
       </c>
       <c r="P7" s="62">
         <f ca="1">O7+1</f>
-        <v>44674</v>
+        <v>44687</v>
       </c>
       <c r="Q7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44675</v>
+        <v>44688</v>
       </c>
       <c r="R7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44676</v>
+        <v>44689</v>
       </c>
       <c r="S7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44677</v>
+        <v>44690</v>
       </c>
       <c r="T7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44678</v>
+        <v>44691</v>
       </c>
       <c r="U7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44679</v>
+        <v>44692</v>
       </c>
       <c r="V7" s="62">
         <f ca="1">U7+1</f>
-        <v>44680</v>
+        <v>44693</v>
       </c>
       <c r="W7" s="62">
         <f ca="1">V7+1</f>
-        <v>44681</v>
+        <v>44694</v>
       </c>
       <c r="X7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44682</v>
+        <v>44695</v>
       </c>
       <c r="Y7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44683</v>
+        <v>44696</v>
       </c>
       <c r="Z7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44684</v>
+        <v>44697</v>
       </c>
       <c r="AA7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44685</v>
+        <v>44698</v>
       </c>
       <c r="AB7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44686</v>
+        <v>44699</v>
       </c>
       <c r="AC7" s="62">
         <f ca="1">AB7+1</f>
-        <v>44687</v>
+        <v>44700</v>
       </c>
       <c r="AD7" s="62">
         <f ca="1">AC7+1</f>
-        <v>44688</v>
+        <v>44701</v>
       </c>
       <c r="AE7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44689</v>
+        <v>44702</v>
       </c>
       <c r="AF7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44690</v>
+        <v>44703</v>
       </c>
       <c r="AG7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44691</v>
+        <v>44704</v>
       </c>
       <c r="AH7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44692</v>
+        <v>44705</v>
       </c>
       <c r="AI7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44693</v>
+        <v>44706</v>
       </c>
       <c r="AJ7" s="62">
         <f ca="1">AI7+1</f>
-        <v>44694</v>
+        <v>44707</v>
       </c>
       <c r="AK7" s="62">
         <f ca="1">AJ7+1</f>
-        <v>44695</v>
+        <v>44708</v>
       </c>
       <c r="AL7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44696</v>
+        <v>44709</v>
       </c>
       <c r="AM7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44697</v>
+        <v>44710</v>
       </c>
       <c r="AN7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44698</v>
+        <v>44711</v>
       </c>
       <c r="AO7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44699</v>
+        <v>44712</v>
       </c>
       <c r="AP7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44700</v>
+        <v>44713</v>
       </c>
       <c r="AQ7" s="62">
         <f ca="1">AP7+1</f>
-        <v>44701</v>
+        <v>44714</v>
       </c>
       <c r="AR7" s="62">
         <f ca="1">AQ7+1</f>
-        <v>44702</v>
+        <v>44715</v>
       </c>
       <c r="AS7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44703</v>
+        <v>44716</v>
       </c>
       <c r="AT7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44704</v>
+        <v>44717</v>
       </c>
       <c r="AU7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44705</v>
+        <v>44718</v>
       </c>
       <c r="AV7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44706</v>
+        <v>44719</v>
       </c>
       <c r="AW7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44707</v>
+        <v>44720</v>
       </c>
       <c r="AX7" s="62">
         <f ca="1">AW7+1</f>
-        <v>44708</v>
+        <v>44721</v>
       </c>
       <c r="AY7" s="62">
         <f ca="1">AX7+1</f>
-        <v>44709</v>
+        <v>44722</v>
       </c>
       <c r="AZ7" s="62">
         <f t="shared" ref="AZ7:BD7" ca="1" si="1">AY7+1</f>
-        <v>44710</v>
+        <v>44723</v>
       </c>
       <c r="BA7" s="62">
         <f t="shared" ca="1" si="1"/>
-        <v>44711</v>
+        <v>44724</v>
       </c>
       <c r="BB7" s="62">
         <f t="shared" ca="1" si="1"/>
-        <v>44712</v>
+        <v>44725</v>
       </c>
       <c r="BC7" s="62">
         <f t="shared" ca="1" si="1"/>
-        <v>44713</v>
+        <v>44726</v>
       </c>
       <c r="BD7" s="62">
         <f t="shared" ca="1" si="1"/>
-        <v>44714</v>
+        <v>44727</v>
       </c>
       <c r="BE7" s="62">
         <f ca="1">BD7+1</f>
-        <v>44715</v>
+        <v>44728</v>
       </c>
       <c r="BF7" s="62">
         <f ca="1">BE7+1</f>
-        <v>44716</v>
+        <v>44729</v>
       </c>
       <c r="BG7" s="62">
         <f t="shared" ref="BG7:BK7" ca="1" si="2">BF7+1</f>
-        <v>44717</v>
+        <v>44730</v>
       </c>
       <c r="BH7" s="62">
         <f t="shared" ca="1" si="2"/>
-        <v>44718</v>
+        <v>44731</v>
       </c>
       <c r="BI7" s="62">
         <f t="shared" ca="1" si="2"/>
-        <v>44719</v>
+        <v>44732</v>
       </c>
       <c r="BJ7" s="62">
         <f t="shared" ca="1" si="2"/>
-        <v>44720</v>
+        <v>44733</v>
       </c>
       <c r="BK7" s="77">
         <f t="shared" ca="1" si="2"/>
-        <v>44721</v>
+        <v>44734</v>
       </c>
     </row>
     <row r="8" spans="1:63" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -7242,7 +7242,7 @@
       <c r="G8" s="79"/>
       <c r="H8" s="63" t="str">
         <f ca="1">LEFT(TEXT(H7,"ddd"),1)</f>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="I8" s="60" t="str">
         <f ca="1">LEFT(TEXT(I7,"ddd"),1)</f>
@@ -7250,19 +7250,19 @@
       </c>
       <c r="J8" s="60" t="str">
         <f ca="1">LEFT(TEXT(J7,"ddd"),1)</f>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="K8" s="60" t="str">
         <f t="shared" ref="K8:BK8" ca="1" si="3">LEFT(TEXT(K7,"ddd"),1)</f>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="L8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="M8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="N8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7270,7 +7270,7 @@
       </c>
       <c r="O8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="P8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7278,19 +7278,19 @@
       </c>
       <c r="Q8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="R8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="S8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="T8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="U8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7298,7 +7298,7 @@
       </c>
       <c r="V8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="W8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7306,19 +7306,19 @@
       </c>
       <c r="X8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="Y8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="Z8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AA8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="AB8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7326,7 +7326,7 @@
       </c>
       <c r="AC8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AD8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7334,19 +7334,19 @@
       </c>
       <c r="AE8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="AF8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AG8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AH8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="AI8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7354,7 +7354,7 @@
       </c>
       <c r="AJ8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AK8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7362,19 +7362,19 @@
       </c>
       <c r="AL8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="AM8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AN8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AO8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="AP8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7382,7 +7382,7 @@
       </c>
       <c r="AQ8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AR8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7390,19 +7390,19 @@
       </c>
       <c r="AS8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="AT8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AU8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AV8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="AW8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7410,7 +7410,7 @@
       </c>
       <c r="AX8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AY8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7418,19 +7418,19 @@
       </c>
       <c r="AZ8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="BA8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="BB8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="BC8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="BD8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7438,7 +7438,7 @@
       </c>
       <c r="BE8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="BF8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7446,19 +7446,19 @@
       </c>
       <c r="BG8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="BH8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="BI8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="BJ8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="BK8" s="78" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7774,7 +7774,7 @@
       </c>
       <c r="E11" s="51">
         <f ca="1">TODAY()</f>
-        <v>44656</v>
+        <v>44669</v>
       </c>
       <c r="F11" s="49">
         <v>3</v>
@@ -8014,7 +8014,7 @@
       <c r="D12" s="53"/>
       <c r="E12" s="51">
         <f ca="1">TODAY()+5</f>
-        <v>44661</v>
+        <v>44674</v>
       </c>
       <c r="F12" s="49">
         <v>1</v>
@@ -8256,7 +8256,7 @@
       </c>
       <c r="E13" s="51">
         <f ca="1">TODAY()-3</f>
-        <v>44653</v>
+        <v>44666</v>
       </c>
       <c r="F13" s="49">
         <v>10</v>
@@ -8496,7 +8496,7 @@
       <c r="D14" s="53"/>
       <c r="E14" s="51">
         <f ca="1">TODAY()+20</f>
-        <v>44676</v>
+        <v>44689</v>
       </c>
       <c r="F14" s="49">
         <v>1</v>
@@ -8738,7 +8738,7 @@
       </c>
       <c r="E15" s="51">
         <f ca="1">TODAY()+6</f>
-        <v>44662</v>
+        <v>44675</v>
       </c>
       <c r="F15" s="49">
         <v>6</v>
@@ -9215,7 +9215,7 @@
       </c>
       <c r="E17" s="51">
         <f ca="1">TODAY()+6</f>
-        <v>44662</v>
+        <v>44675</v>
       </c>
       <c r="F17" s="49">
         <v>13</v>
@@ -9457,7 +9457,7 @@
       </c>
       <c r="E18" s="51">
         <f ca="1">TODAY()+7</f>
-        <v>44663</v>
+        <v>44676</v>
       </c>
       <c r="F18" s="49">
         <v>9</v>
@@ -9699,7 +9699,7 @@
       </c>
       <c r="E19" s="51">
         <f ca="1">TODAY()+15</f>
-        <v>44671</v>
+        <v>44684</v>
       </c>
       <c r="F19" s="49">
         <v>11</v>
@@ -9939,7 +9939,7 @@
       <c r="D20" s="53"/>
       <c r="E20" s="51">
         <f ca="1">TODAY()+24</f>
-        <v>44680</v>
+        <v>44693</v>
       </c>
       <c r="F20" s="49">
         <v>1</v>
@@ -10179,7 +10179,7 @@
       <c r="D21" s="104"/>
       <c r="E21" s="51">
         <f ca="1">TODAY()+25</f>
-        <v>44681</v>
+        <v>44694</v>
       </c>
       <c r="F21" s="49">
         <v>24</v>
@@ -10654,7 +10654,7 @@
       <c r="D23" s="104"/>
       <c r="E23" s="51">
         <f ca="1">TODAY()+15</f>
-        <v>44671</v>
+        <v>44684</v>
       </c>
       <c r="F23" s="49">
         <v>4</v>
@@ -10894,7 +10894,7 @@
       <c r="D24" s="53"/>
       <c r="E24" s="51">
         <f ca="1">TODAY()+19</f>
-        <v>44675</v>
+        <v>44688</v>
       </c>
       <c r="F24" s="49">
         <v>14</v>
@@ -11134,7 +11134,7 @@
       <c r="D25" s="104"/>
       <c r="E25" s="51">
         <f ca="1">TODAY()+35</f>
-        <v>44691</v>
+        <v>44704</v>
       </c>
       <c r="F25" s="49">
         <v>6</v>
@@ -11374,7 +11374,7 @@
       <c r="D26" s="53"/>
       <c r="E26" s="51">
         <f ca="1">TODAY()+48</f>
-        <v>44704</v>
+        <v>44717</v>
       </c>
       <c r="F26" s="49">
         <v>3</v>
@@ -11614,7 +11614,7 @@
       <c r="D27" s="104"/>
       <c r="E27" s="51">
         <f ca="1">TODAY()+40</f>
-        <v>44696</v>
+        <v>44709</v>
       </c>
       <c r="F27" s="49">
         <v>19</v>
@@ -12089,7 +12089,7 @@
       <c r="D29" s="104"/>
       <c r="E29" s="51">
         <f ca="1">TODAY()+37</f>
-        <v>44693</v>
+        <v>44706</v>
       </c>
       <c r="F29" s="49">
         <v>15</v>
@@ -12329,7 +12329,7 @@
       <c r="D30" s="53"/>
       <c r="E30" s="51">
         <f ca="1">TODAY()+29</f>
-        <v>44685</v>
+        <v>44698</v>
       </c>
       <c r="F30" s="49">
         <v>5</v>
@@ -12569,7 +12569,7 @@
       <c r="D31" s="104"/>
       <c r="E31" s="51">
         <f ca="1">TODAY()+80</f>
-        <v>44736</v>
+        <v>44749</v>
       </c>
       <c r="F31" s="49">
         <v>5</v>
@@ -13958,7 +13958,7 @@
       </c>
       <c r="C5" s="56">
         <f ca="1">IFERROR(IF(MIN(Milestones[Start])=0,TODAY(),MIN(Milestones[Start])),TODAY())</f>
-        <v>44653</v>
+        <v>44666</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="73"/>
@@ -13971,14 +13971,14 @@
       <c r="L5" s="43"/>
       <c r="M5" s="44"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="119" t="s">
+      <c r="O5" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="119"/>
-      <c r="Q5" s="119"/>
-      <c r="R5" s="119"/>
-      <c r="S5" s="119"/>
-      <c r="T5" s="119"/>
+      <c r="P5" s="122"/>
+      <c r="Q5" s="122"/>
+      <c r="R5" s="122"/>
+      <c r="S5" s="122"/>
+      <c r="T5" s="122"/>
       <c r="U5" s="57">
         <v>13</v>
       </c>
@@ -14051,7 +14051,7 @@
       <c r="N6" s="29"/>
       <c r="O6" s="29" t="str">
         <f ca="1">IF(TEXT(O7,"mmmm")=H6,"",TEXT(O7,"mmmm"))</f>
-        <v/>
+        <v>maio</v>
       </c>
       <c r="P6" s="29"/>
       <c r="Q6" s="29"/>
@@ -14071,7 +14071,7 @@
       <c r="AB6" s="29"/>
       <c r="AC6" s="29" t="str">
         <f ca="1">IF(OR(TEXT(AC7,"mmmm")=V6,TEXT(AC7,"mmmm")=O6,TEXT(AC7,"mmmm")=H6),"",TEXT(AC7,"mmmm"))</f>
-        <v>maio</v>
+        <v/>
       </c>
       <c r="AD6" s="29"/>
       <c r="AE6" s="29"/>
@@ -14091,7 +14091,7 @@
       <c r="AP6" s="29"/>
       <c r="AQ6" s="29" t="str">
         <f ca="1">IF(OR(TEXT(AQ7,"mmmm")=AJ6,TEXT(AQ7,"mmmm")=AC6,TEXT(AQ7,"mmmm")=V6,TEXT(AQ7,"mmmm")=O6),"",TEXT(AQ7,"mmmm"))</f>
-        <v/>
+        <v>junho</v>
       </c>
       <c r="AR6" s="29"/>
       <c r="AS6" s="29"/>
@@ -14111,7 +14111,7 @@
       <c r="BD6" s="29"/>
       <c r="BE6" s="29" t="str">
         <f ca="1">IF(OR(TEXT(BE7,"mmmm")=AX6,TEXT(BE7,"mmmm")=AQ6,TEXT(BE7,"mmmm")=AJ6,TEXT(BE7,"mmmm")=AC6),"",TEXT(BE7,"mmmm"))</f>
-        <v>junho</v>
+        <v/>
       </c>
       <c r="BF6" s="29"/>
       <c r="BG6" s="29"/>
@@ -14129,227 +14129,227 @@
       <c r="G7" s="23"/>
       <c r="H7" s="64">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>44666</v>
+        <v>44679</v>
       </c>
       <c r="I7" s="66">
         <f ca="1">H7+1</f>
-        <v>44667</v>
+        <v>44680</v>
       </c>
       <c r="J7" s="66">
         <f t="shared" ref="J7:AW7" ca="1" si="0">I7+1</f>
-        <v>44668</v>
+        <v>44681</v>
       </c>
       <c r="K7" s="66">
         <f ca="1">J7+1</f>
-        <v>44669</v>
+        <v>44682</v>
       </c>
       <c r="L7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44670</v>
+        <v>44683</v>
       </c>
       <c r="M7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44671</v>
+        <v>44684</v>
       </c>
       <c r="N7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44672</v>
+        <v>44685</v>
       </c>
       <c r="O7" s="66">
         <f ca="1">N7+1</f>
-        <v>44673</v>
+        <v>44686</v>
       </c>
       <c r="P7" s="66">
         <f ca="1">O7+1</f>
-        <v>44674</v>
+        <v>44687</v>
       </c>
       <c r="Q7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44675</v>
+        <v>44688</v>
       </c>
       <c r="R7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44676</v>
+        <v>44689</v>
       </c>
       <c r="S7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44677</v>
+        <v>44690</v>
       </c>
       <c r="T7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44678</v>
+        <v>44691</v>
       </c>
       <c r="U7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44679</v>
+        <v>44692</v>
       </c>
       <c r="V7" s="66">
         <f ca="1">U7+1</f>
-        <v>44680</v>
+        <v>44693</v>
       </c>
       <c r="W7" s="66">
         <f ca="1">V7+1</f>
-        <v>44681</v>
+        <v>44694</v>
       </c>
       <c r="X7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44682</v>
+        <v>44695</v>
       </c>
       <c r="Y7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44683</v>
+        <v>44696</v>
       </c>
       <c r="Z7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44684</v>
+        <v>44697</v>
       </c>
       <c r="AA7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44685</v>
+        <v>44698</v>
       </c>
       <c r="AB7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44686</v>
+        <v>44699</v>
       </c>
       <c r="AC7" s="66">
         <f ca="1">AB7+1</f>
-        <v>44687</v>
+        <v>44700</v>
       </c>
       <c r="AD7" s="66">
         <f ca="1">AC7+1</f>
-        <v>44688</v>
+        <v>44701</v>
       </c>
       <c r="AE7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44689</v>
+        <v>44702</v>
       </c>
       <c r="AF7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44690</v>
+        <v>44703</v>
       </c>
       <c r="AG7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44691</v>
+        <v>44704</v>
       </c>
       <c r="AH7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44692</v>
+        <v>44705</v>
       </c>
       <c r="AI7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44693</v>
+        <v>44706</v>
       </c>
       <c r="AJ7" s="66">
         <f ca="1">AI7+1</f>
-        <v>44694</v>
+        <v>44707</v>
       </c>
       <c r="AK7" s="66">
         <f ca="1">AJ7+1</f>
-        <v>44695</v>
+        <v>44708</v>
       </c>
       <c r="AL7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44696</v>
+        <v>44709</v>
       </c>
       <c r="AM7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44697</v>
+        <v>44710</v>
       </c>
       <c r="AN7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44698</v>
+        <v>44711</v>
       </c>
       <c r="AO7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44699</v>
+        <v>44712</v>
       </c>
       <c r="AP7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44700</v>
+        <v>44713</v>
       </c>
       <c r="AQ7" s="66">
         <f ca="1">AP7+1</f>
-        <v>44701</v>
+        <v>44714</v>
       </c>
       <c r="AR7" s="66">
         <f ca="1">AQ7+1</f>
-        <v>44702</v>
+        <v>44715</v>
       </c>
       <c r="AS7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44703</v>
+        <v>44716</v>
       </c>
       <c r="AT7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44704</v>
+        <v>44717</v>
       </c>
       <c r="AU7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44705</v>
+        <v>44718</v>
       </c>
       <c r="AV7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44706</v>
+        <v>44719</v>
       </c>
       <c r="AW7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44707</v>
+        <v>44720</v>
       </c>
       <c r="AX7" s="66">
         <f ca="1">AW7+1</f>
-        <v>44708</v>
+        <v>44721</v>
       </c>
       <c r="AY7" s="66">
         <f ca="1">AX7+1</f>
-        <v>44709</v>
+        <v>44722</v>
       </c>
       <c r="AZ7" s="66">
         <f t="shared" ref="AZ7:BD7" ca="1" si="1">AY7+1</f>
-        <v>44710</v>
+        <v>44723</v>
       </c>
       <c r="BA7" s="66">
         <f t="shared" ca="1" si="1"/>
-        <v>44711</v>
+        <v>44724</v>
       </c>
       <c r="BB7" s="66">
         <f t="shared" ca="1" si="1"/>
-        <v>44712</v>
+        <v>44725</v>
       </c>
       <c r="BC7" s="66">
         <f t="shared" ca="1" si="1"/>
-        <v>44713</v>
+        <v>44726</v>
       </c>
       <c r="BD7" s="66">
         <f t="shared" ca="1" si="1"/>
-        <v>44714</v>
+        <v>44727</v>
       </c>
       <c r="BE7" s="66">
         <f ca="1">BD7+1</f>
-        <v>44715</v>
+        <v>44728</v>
       </c>
       <c r="BF7" s="66">
         <f ca="1">BE7+1</f>
-        <v>44716</v>
+        <v>44729</v>
       </c>
       <c r="BG7" s="66">
         <f t="shared" ref="BG7:BK7" ca="1" si="2">BF7+1</f>
-        <v>44717</v>
+        <v>44730</v>
       </c>
       <c r="BH7" s="66">
         <f t="shared" ca="1" si="2"/>
-        <v>44718</v>
+        <v>44731</v>
       </c>
       <c r="BI7" s="66">
         <f t="shared" ca="1" si="2"/>
-        <v>44719</v>
+        <v>44732</v>
       </c>
       <c r="BJ7" s="66">
         <f t="shared" ca="1" si="2"/>
-        <v>44720</v>
+        <v>44733</v>
       </c>
       <c r="BK7" s="30">
         <f t="shared" ca="1" si="2"/>
-        <v>44721</v>
+        <v>44734</v>
       </c>
     </row>
     <row r="8" spans="1:63" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -14372,7 +14372,7 @@
       <c r="G8" s="69"/>
       <c r="H8" s="68" t="str">
         <f ca="1">LEFT(TEXT(H7,"ddd"),1)</f>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="I8" s="67" t="str">
         <f ca="1">LEFT(TEXT(I7,"ddd"),1)</f>
@@ -14380,19 +14380,19 @@
       </c>
       <c r="J8" s="67" t="str">
         <f ca="1">LEFT(TEXT(J7,"ddd"),1)</f>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="K8" s="67" t="str">
         <f t="shared" ref="K8:AM8" ca="1" si="3">LEFT(TEXT(K7,"ddd"),1)</f>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="L8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="M8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="N8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -14400,7 +14400,7 @@
       </c>
       <c r="O8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="P8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -14408,19 +14408,19 @@
       </c>
       <c r="Q8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="R8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="S8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="T8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="U8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -14428,7 +14428,7 @@
       </c>
       <c r="V8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="W8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -14436,19 +14436,19 @@
       </c>
       <c r="X8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="Y8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="Z8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AA8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="AB8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -14456,7 +14456,7 @@
       </c>
       <c r="AC8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AD8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -14464,19 +14464,19 @@
       </c>
       <c r="AE8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="AF8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AG8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AH8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="AI8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -14484,7 +14484,7 @@
       </c>
       <c r="AJ8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AK8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -14492,19 +14492,19 @@
       </c>
       <c r="AL8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="AM8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AN8" s="67" t="str">
         <f t="shared" ref="AN8:BK8" ca="1" si="4">LEFT(TEXT(AN7,"ddd"),1)</f>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AO8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="AP8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -14512,7 +14512,7 @@
       </c>
       <c r="AQ8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AR8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -14520,19 +14520,19 @@
       </c>
       <c r="AS8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="AT8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AU8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AV8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="AW8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -14540,7 +14540,7 @@
       </c>
       <c r="AX8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AY8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -14548,19 +14548,19 @@
       </c>
       <c r="AZ8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="BA8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="BB8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="BC8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="BD8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -14568,7 +14568,7 @@
       </c>
       <c r="BE8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="BF8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -14576,19 +14576,19 @@
       </c>
       <c r="BG8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>s</v>
       </c>
       <c r="BH8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="BI8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="BJ8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="BK8" s="65" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -14905,7 +14905,7 @@
       </c>
       <c r="E11" s="51">
         <f ca="1">TODAY()</f>
-        <v>44656</v>
+        <v>44669</v>
       </c>
       <c r="F11" s="49">
         <v>3</v>
@@ -15145,7 +15145,7 @@
       <c r="D12" s="52"/>
       <c r="E12" s="51">
         <f ca="1">TODAY()+5</f>
-        <v>44661</v>
+        <v>44674</v>
       </c>
       <c r="F12" s="49">
         <v>1</v>
@@ -15387,7 +15387,7 @@
       </c>
       <c r="E13" s="51">
         <f ca="1">TODAY()-3</f>
-        <v>44653</v>
+        <v>44666</v>
       </c>
       <c r="F13" s="49">
         <v>10</v>
@@ -15627,7 +15627,7 @@
       <c r="D14" s="52"/>
       <c r="E14" s="51">
         <f ca="1">TODAY()+20</f>
-        <v>44676</v>
+        <v>44689</v>
       </c>
       <c r="F14" s="49">
         <v>1</v>
@@ -15869,7 +15869,7 @@
       </c>
       <c r="E15" s="51">
         <f ca="1">TODAY()+6</f>
-        <v>44662</v>
+        <v>44675</v>
       </c>
       <c r="F15" s="49">
         <v>6</v>
@@ -16346,7 +16346,7 @@
       </c>
       <c r="E17" s="51">
         <f ca="1">TODAY()+6</f>
-        <v>44662</v>
+        <v>44675</v>
       </c>
       <c r="F17" s="49">
         <v>13</v>
@@ -16588,7 +16588,7 @@
       </c>
       <c r="E18" s="51">
         <f ca="1">TODAY()+7</f>
-        <v>44663</v>
+        <v>44676</v>
       </c>
       <c r="F18" s="49">
         <v>9</v>
@@ -16830,7 +16830,7 @@
       </c>
       <c r="E19" s="51">
         <f ca="1">TODAY()+15</f>
-        <v>44671</v>
+        <v>44684</v>
       </c>
       <c r="F19" s="49">
         <v>11</v>
@@ -17070,7 +17070,7 @@
       <c r="D20" s="52"/>
       <c r="E20" s="51">
         <f ca="1">TODAY()+24</f>
-        <v>44680</v>
+        <v>44693</v>
       </c>
       <c r="F20" s="49">
         <v>1</v>
@@ -17310,7 +17310,7 @@
       <c r="D21" s="52"/>
       <c r="E21" s="51">
         <f ca="1">TODAY()+25</f>
-        <v>44681</v>
+        <v>44694</v>
       </c>
       <c r="F21" s="49">
         <v>24</v>
@@ -17785,7 +17785,7 @@
       <c r="D23" s="52"/>
       <c r="E23" s="51">
         <f ca="1">TODAY()+15</f>
-        <v>44671</v>
+        <v>44684</v>
       </c>
       <c r="F23" s="49">
         <v>4</v>
@@ -18025,7 +18025,7 @@
       <c r="D24" s="52"/>
       <c r="E24" s="51">
         <f ca="1">TODAY()+19</f>
-        <v>44675</v>
+        <v>44688</v>
       </c>
       <c r="F24" s="49">
         <v>14</v>
@@ -18265,7 +18265,7 @@
       <c r="D25" s="52"/>
       <c r="E25" s="51">
         <f ca="1">TODAY()+35</f>
-        <v>44691</v>
+        <v>44704</v>
       </c>
       <c r="F25" s="49">
         <v>6</v>
@@ -18505,7 +18505,7 @@
       <c r="D26" s="52"/>
       <c r="E26" s="51">
         <f ca="1">TODAY()+48</f>
-        <v>44704</v>
+        <v>44717</v>
       </c>
       <c r="F26" s="49">
         <v>3</v>
@@ -18745,7 +18745,7 @@
       <c r="D27" s="52"/>
       <c r="E27" s="51">
         <f ca="1">TODAY()+40</f>
-        <v>44696</v>
+        <v>44709</v>
       </c>
       <c r="F27" s="49">
         <v>19</v>
@@ -19220,7 +19220,7 @@
       <c r="D29" s="52"/>
       <c r="E29" s="51">
         <f ca="1">TODAY()+37</f>
-        <v>44693</v>
+        <v>44706</v>
       </c>
       <c r="F29" s="49">
         <v>15</v>
@@ -19460,7 +19460,7 @@
       <c r="D30" s="52"/>
       <c r="E30" s="51">
         <f ca="1">TODAY()+29</f>
-        <v>44685</v>
+        <v>44698</v>
       </c>
       <c r="F30" s="49">
         <v>5</v>
@@ -19700,7 +19700,7 @@
       <c r="D31" s="52"/>
       <c r="E31" s="51">
         <f ca="1">TODAY()+80</f>
-        <v>44736</v>
+        <v>44749</v>
       </c>
       <c r="F31" s="49">
         <v>5</v>

</xml_diff>

<commit_message>
Alterando a cor do grafico de GRAANT para ficar de acordo com o tema do nosso grupo
</commit_message>
<xml_diff>
--- a/Documentação/Date tracking Gantt chart1.xlsx
+++ b/Documentação/Date tracking Gantt chart1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E30BBE-F719-4DB1-AB81-838C4AFF6D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C921BD3-ADF7-4CB8-8B3A-9560D5840E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -17,15 +17,15 @@
     <definedName name="Milestone_Marker" localSheetId="2">Blue!$C$6</definedName>
     <definedName name="Milestone_Marker" localSheetId="1">Green!$C$6</definedName>
     <definedName name="Milestone_Marker">Purple!$C$6</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">Blue!$6:$8</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">Green!$6:$8</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="3">Purple!$6:$8</definedName>
     <definedName name="Project_Start" localSheetId="2">Blue!$C$5</definedName>
     <definedName name="Project_Start" localSheetId="1">Green!$C$5</definedName>
     <definedName name="Project_Start">Purple!$C$5</definedName>
     <definedName name="Scrolling_Increment" localSheetId="2">Blue!$U$5</definedName>
     <definedName name="Scrolling_Increment" localSheetId="1">Green!$U$5</definedName>
     <definedName name="Scrolling_Increment">Purple!$U$5</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">Blue!$6:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">Green!$6:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">Purple!$6:$8</definedName>
     <definedName name="Today" localSheetId="2">TODAY()</definedName>
     <definedName name="Today" localSheetId="1">TODAY()</definedName>
     <definedName name="Today" localSheetId="3">TODAY()</definedName>
@@ -1180,18 +1180,18 @@
     </xf>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Comma [0]" xfId="10" builtinId="6" customBuiltin="1"/>
     <cellStyle name="Date" xfId="9" xr:uid="{229918B6-DD13-4F5A-97B9-305F7E002AA3}"/>
-    <cellStyle name="Explanatory Text" xfId="12" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Porcentagem" xfId="2" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Separador de milhares [0]" xfId="10" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Texto Explicativo" xfId="12" builtinId="53"/>
+    <cellStyle name="Título" xfId="5" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="6" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="7" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="8" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Título 4" xfId="11" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Vírgula" xfId="4" builtinId="3" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
   <dxfs count="26">
@@ -1914,42 +1914,42 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Attitude">
   <a:themeElements>
-    <a:clrScheme name="Cool Chart Colors">
+    <a:clrScheme name="Personalizada 1">
       <a:dk1>
-        <a:srgbClr val="122173"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="8439BD"/>
+        <a:srgbClr val="632E62"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="EAE5EB"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="0EABB7"/>
+        <a:srgbClr val="92278F"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="4868E5"/>
+        <a:srgbClr val="9B57D3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="20A472"/>
+        <a:srgbClr val="755DD9"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="B13DC8"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="172DA6"/>
+        <a:srgbClr val="45A5ED"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="00B0F0"/>
+        <a:srgbClr val="5982DB"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="00B0F0"/>
+        <a:srgbClr val="0066FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="B036B3"/>
+        <a:srgbClr val="666699"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Calibri">
@@ -2248,8 +2248,8 @@
   </sheetPr>
   <dimension ref="A1:BK33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="C5" s="56">
         <f ca="1">IFERROR(IF(MIN(Milestones34[Start])=0,TODAY(),MIN(Milestones34[Start])),TODAY())</f>
-        <v>44629</v>
+        <v>44632</v>
       </c>
       <c r="E5" s="73"/>
       <c r="H5" s="36"/>
@@ -2482,7 +2482,7 @@
       <c r="AB6" s="29"/>
       <c r="AC6" s="29" t="str">
         <f ca="1">IF(OR(TEXT(AC7,"mmmm")=V6,TEXT(AC7,"mmmm")=O6,TEXT(AC7,"mmmm")=H6),"",TEXT(AC7,"mmmm"))</f>
-        <v/>
+        <v>abril</v>
       </c>
       <c r="AD6" s="29"/>
       <c r="AE6" s="29"/>
@@ -2525,139 +2525,139 @@
       <c r="G7" s="23"/>
       <c r="H7" s="109">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>44629</v>
+        <v>44632</v>
       </c>
       <c r="I7" s="110">
         <f ca="1">H7+1</f>
-        <v>44630</v>
+        <v>44633</v>
       </c>
       <c r="J7" s="110">
         <f t="shared" ref="J7:AB7" ca="1" si="0">I7+1</f>
-        <v>44631</v>
+        <v>44634</v>
       </c>
       <c r="K7" s="110">
         <f ca="1">J7+1</f>
-        <v>44632</v>
+        <v>44635</v>
       </c>
       <c r="L7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44633</v>
+        <v>44636</v>
       </c>
       <c r="M7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44634</v>
+        <v>44637</v>
       </c>
       <c r="N7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44635</v>
+        <v>44638</v>
       </c>
       <c r="O7" s="110">
         <f ca="1">N7+1</f>
-        <v>44636</v>
+        <v>44639</v>
       </c>
       <c r="P7" s="110">
         <f ca="1">O7+1</f>
-        <v>44637</v>
+        <v>44640</v>
       </c>
       <c r="Q7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44638</v>
+        <v>44641</v>
       </c>
       <c r="R7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44639</v>
+        <v>44642</v>
       </c>
       <c r="S7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44640</v>
+        <v>44643</v>
       </c>
       <c r="T7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44641</v>
+        <v>44644</v>
       </c>
       <c r="U7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44642</v>
+        <v>44645</v>
       </c>
       <c r="V7" s="110">
         <f ca="1">U7+1</f>
-        <v>44643</v>
+        <v>44646</v>
       </c>
       <c r="W7" s="110">
         <f ca="1">V7+1</f>
-        <v>44644</v>
+        <v>44647</v>
       </c>
       <c r="X7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44645</v>
+        <v>44648</v>
       </c>
       <c r="Y7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44646</v>
+        <v>44649</v>
       </c>
       <c r="Z7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44647</v>
+        <v>44650</v>
       </c>
       <c r="AA7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44648</v>
+        <v>44651</v>
       </c>
       <c r="AB7" s="110">
         <f t="shared" ca="1" si="0"/>
-        <v>44649</v>
+        <v>44652</v>
       </c>
       <c r="AC7" s="110">
         <f ca="1">AB7+1</f>
-        <v>44650</v>
+        <v>44653</v>
       </c>
       <c r="AD7" s="119">
         <f ca="1">AC7+1</f>
-        <v>44651</v>
+        <v>44654</v>
       </c>
       <c r="AE7" s="110">
         <f t="shared" ref="AE7" ca="1" si="1">AD7+1</f>
-        <v>44652</v>
+        <v>44655</v>
       </c>
       <c r="AF7" s="110">
         <f t="shared" ref="AF7" ca="1" si="2">AE7+1</f>
-        <v>44653</v>
+        <v>44656</v>
       </c>
       <c r="AG7" s="110">
         <f t="shared" ref="AG7" ca="1" si="3">AF7+1</f>
-        <v>44654</v>
+        <v>44657</v>
       </c>
       <c r="AH7" s="110">
         <f t="shared" ref="AH7" ca="1" si="4">AG7+1</f>
-        <v>44655</v>
+        <v>44658</v>
       </c>
       <c r="AI7" s="110">
         <f t="shared" ref="AI7" ca="1" si="5">AH7+1</f>
-        <v>44656</v>
+        <v>44659</v>
       </c>
       <c r="AJ7" s="110">
         <f ca="1">AI7+1</f>
-        <v>44657</v>
+        <v>44660</v>
       </c>
       <c r="AK7" s="110">
         <f ca="1">AJ7+1</f>
-        <v>44658</v>
+        <v>44661</v>
       </c>
       <c r="AL7" s="110">
         <f ca="1">AK7+1</f>
-        <v>44659</v>
+        <v>44662</v>
       </c>
       <c r="AM7" s="110">
         <f ca="1">AL7+1</f>
-        <v>44660</v>
+        <v>44663</v>
       </c>
       <c r="AN7" s="110">
         <f t="shared" ref="AN7" ca="1" si="6">AM7+1</f>
-        <v>44661</v>
+        <v>44664</v>
       </c>
       <c r="AO7" s="110">
         <f t="shared" ref="AO7" ca="1" si="7">AN7+1</f>
-        <v>44662</v>
+        <v>44665</v>
       </c>
       <c r="AP7" s="110"/>
       <c r="AQ7" s="110"/>
@@ -2702,11 +2702,11 @@
       <c r="G8" s="115"/>
       <c r="H8" s="106" t="str">
         <f ca="1">LEFT(TEXT(H7,"ddd"),1)</f>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="I8" s="107" t="str">
         <f ca="1">LEFT(TEXT(I7,"ddd"),1)</f>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="J8" s="107" t="str">
         <f ca="1">LEFT(TEXT(J7,"ddd"),1)</f>
@@ -2714,27 +2714,27 @@
       </c>
       <c r="K8" s="107" t="str">
         <f t="shared" ref="K8:AC8" ca="1" si="8">LEFT(TEXT(K7,"ddd"),1)</f>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="L8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="M8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="N8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="O8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="P8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="Q8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -2742,27 +2742,27 @@
       </c>
       <c r="R8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="S8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="T8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="U8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="V8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="W8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="X8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -2770,27 +2770,27 @@
       </c>
       <c r="Y8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="Z8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="AA8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AB8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AC8" s="107" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AD8" s="120" t="str">
         <f t="shared" ref="AD8:AJ8" ca="1" si="9">LEFT(TEXT(AD7,"ddd"),1)</f>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="AE8" s="107" t="str">
         <f t="shared" ca="1" si="9"/>
@@ -2798,27 +2798,27 @@
       </c>
       <c r="AF8" s="107" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="AG8" s="107" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="AH8" s="107" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AI8" s="107" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AJ8" s="107" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AK8" s="107" t="str">
         <f t="shared" ref="AK8:AL8" ca="1" si="10">LEFT(TEXT(AK7,"ddd"),1)</f>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="AL8" s="107" t="str">
         <f t="shared" ca="1" si="10"/>
@@ -2826,15 +2826,15 @@
       </c>
       <c r="AM8" s="107" t="str">
         <f t="shared" ref="AM8:AO8" ca="1" si="11">LEFT(TEXT(AM7,"ddd"),1)</f>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="AN8" s="107" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="AO8" s="107" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AP8" s="107"/>
       <c r="AQ8" s="107"/>
@@ -3102,7 +3102,7 @@
       </c>
       <c r="E11" s="51">
         <f ca="1">TODAY()-40</f>
-        <v>44629</v>
+        <v>44632</v>
       </c>
       <c r="F11" s="49">
         <v>36</v>
@@ -3278,7 +3278,7 @@
       </c>
       <c r="E12" s="51">
         <f ca="1">TODAY()-30</f>
-        <v>44639</v>
+        <v>44642</v>
       </c>
       <c r="F12" s="121">
         <v>15</v>
@@ -3451,7 +3451,7 @@
       </c>
       <c r="E13" s="51">
         <f ca="1">TODAY()-32</f>
-        <v>44637</v>
+        <v>44640</v>
       </c>
       <c r="F13" s="49">
         <v>13</v>
@@ -3627,7 +3627,7 @@
       </c>
       <c r="E14" s="51">
         <f ca="1">TODAY()-19</f>
-        <v>44650</v>
+        <v>44653</v>
       </c>
       <c r="F14" s="49">
         <v>4</v>
@@ -3800,7 +3800,7 @@
       </c>
       <c r="E15" s="51">
         <f ca="1">TODAY()-28</f>
-        <v>44641</v>
+        <v>44644</v>
       </c>
       <c r="F15" s="49">
         <v>9</v>
@@ -4145,7 +4145,7 @@
       </c>
       <c r="E17" s="51">
         <f ca="1">TODAY()-32</f>
-        <v>44637</v>
+        <v>44640</v>
       </c>
       <c r="F17" s="49">
         <v>13</v>
@@ -4321,7 +4321,7 @@
       </c>
       <c r="E18" s="51">
         <f ca="1">TODAY()-29</f>
-        <v>44640</v>
+        <v>44643</v>
       </c>
       <c r="F18" s="49">
         <v>14</v>
@@ -4497,7 +4497,7 @@
       </c>
       <c r="E19" s="51">
         <f ca="1">TODAY()-35</f>
-        <v>44634</v>
+        <v>44637</v>
       </c>
       <c r="F19" s="49">
         <v>10</v>
@@ -4673,7 +4673,7 @@
       </c>
       <c r="E20" s="51">
         <f ca="1">TODAY()-25</f>
-        <v>44644</v>
+        <v>44647</v>
       </c>
       <c r="F20" s="49">
         <v>5</v>
@@ -5015,7 +5015,7 @@
       </c>
       <c r="E22" s="51">
         <f ca="1">TODAY()-30</f>
-        <v>44639</v>
+        <v>44642</v>
       </c>
       <c r="F22" s="49">
         <v>8</v>
@@ -5191,7 +5191,7 @@
       </c>
       <c r="E23" s="51">
         <f ca="1">TODAY()-25</f>
-        <v>44644</v>
+        <v>44647</v>
       </c>
       <c r="F23" s="49">
         <v>8</v>
@@ -5367,7 +5367,7 @@
       </c>
       <c r="E24" s="51">
         <f ca="1">TODAY()-16</f>
-        <v>44653</v>
+        <v>44656</v>
       </c>
       <c r="F24" s="49">
         <v>15</v>
@@ -5543,7 +5543,7 @@
       </c>
       <c r="E25" s="51">
         <f ca="1">TODAY()-28</f>
-        <v>44641</v>
+        <v>44644</v>
       </c>
       <c r="F25" s="49">
         <v>13</v>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="E27" s="51">
         <f ca="1">TODAY()-29</f>
-        <v>44640</v>
+        <v>44643</v>
       </c>
       <c r="F27" s="49">
         <v>15</v>
@@ -6064,7 +6064,7 @@
       </c>
       <c r="E28" s="51">
         <f ca="1">TODAY()-34</f>
-        <v>44635</v>
+        <v>44638</v>
       </c>
       <c r="F28" s="49">
         <v>15</v>
@@ -6240,7 +6240,7 @@
       </c>
       <c r="E29" s="51">
         <f ca="1">TODAY()-40</f>
-        <v>44629</v>
+        <v>44632</v>
       </c>
       <c r="F29" s="49">
         <v>10</v>
@@ -6314,7 +6314,7 @@
       </c>
       <c r="E30" s="51">
         <f ca="1">TODAY()</f>
-        <v>44669</v>
+        <v>44672</v>
       </c>
       <c r="F30" s="49">
         <v>1</v>
@@ -6878,7 +6878,7 @@
       </c>
       <c r="C5" s="56">
         <f ca="1">IFERROR(IF(MIN(Milestones3[Start])=0,TODAY(),MIN(Milestones3[Start])),TODAY())</f>
-        <v>44666</v>
+        <v>44669</v>
       </c>
       <c r="E5" s="73"/>
       <c r="H5" s="39"/>
@@ -6914,7 +6914,7 @@
       </c>
       <c r="H6" s="89" t="str">
         <f ca="1">TEXT(H7,"mmmm")</f>
-        <v>abril</v>
+        <v>maio</v>
       </c>
       <c r="I6" s="89"/>
       <c r="J6" s="89"/>
@@ -6924,7 +6924,7 @@
       <c r="N6" s="29"/>
       <c r="O6" s="29" t="str">
         <f ca="1">IF(TEXT(O7,"mmmm")=H6,"",TEXT(O7,"mmmm"))</f>
-        <v>maio</v>
+        <v/>
       </c>
       <c r="P6" s="29"/>
       <c r="Q6" s="29"/>
@@ -6999,227 +6999,227 @@
       <c r="G7" s="23"/>
       <c r="H7" s="61">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>44679</v>
+        <v>44682</v>
       </c>
       <c r="I7" s="62">
         <f ca="1">H7+1</f>
-        <v>44680</v>
+        <v>44683</v>
       </c>
       <c r="J7" s="62">
         <f t="shared" ref="J7:AW7" ca="1" si="0">I7+1</f>
-        <v>44681</v>
+        <v>44684</v>
       </c>
       <c r="K7" s="62">
         <f ca="1">J7+1</f>
-        <v>44682</v>
+        <v>44685</v>
       </c>
       <c r="L7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44683</v>
+        <v>44686</v>
       </c>
       <c r="M7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44684</v>
+        <v>44687</v>
       </c>
       <c r="N7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44685</v>
+        <v>44688</v>
       </c>
       <c r="O7" s="62">
         <f ca="1">N7+1</f>
-        <v>44686</v>
+        <v>44689</v>
       </c>
       <c r="P7" s="62">
         <f ca="1">O7+1</f>
-        <v>44687</v>
+        <v>44690</v>
       </c>
       <c r="Q7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44688</v>
+        <v>44691</v>
       </c>
       <c r="R7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44689</v>
+        <v>44692</v>
       </c>
       <c r="S7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44690</v>
+        <v>44693</v>
       </c>
       <c r="T7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44691</v>
+        <v>44694</v>
       </c>
       <c r="U7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44692</v>
+        <v>44695</v>
       </c>
       <c r="V7" s="62">
         <f ca="1">U7+1</f>
-        <v>44693</v>
+        <v>44696</v>
       </c>
       <c r="W7" s="62">
         <f ca="1">V7+1</f>
-        <v>44694</v>
+        <v>44697</v>
       </c>
       <c r="X7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44695</v>
+        <v>44698</v>
       </c>
       <c r="Y7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44696</v>
+        <v>44699</v>
       </c>
       <c r="Z7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44697</v>
+        <v>44700</v>
       </c>
       <c r="AA7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44698</v>
+        <v>44701</v>
       </c>
       <c r="AB7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44699</v>
+        <v>44702</v>
       </c>
       <c r="AC7" s="62">
         <f ca="1">AB7+1</f>
-        <v>44700</v>
+        <v>44703</v>
       </c>
       <c r="AD7" s="62">
         <f ca="1">AC7+1</f>
-        <v>44701</v>
+        <v>44704</v>
       </c>
       <c r="AE7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44702</v>
+        <v>44705</v>
       </c>
       <c r="AF7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44703</v>
+        <v>44706</v>
       </c>
       <c r="AG7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44704</v>
+        <v>44707</v>
       </c>
       <c r="AH7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44705</v>
+        <v>44708</v>
       </c>
       <c r="AI7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44706</v>
+        <v>44709</v>
       </c>
       <c r="AJ7" s="62">
         <f ca="1">AI7+1</f>
-        <v>44707</v>
+        <v>44710</v>
       </c>
       <c r="AK7" s="62">
         <f ca="1">AJ7+1</f>
-        <v>44708</v>
+        <v>44711</v>
       </c>
       <c r="AL7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44709</v>
+        <v>44712</v>
       </c>
       <c r="AM7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44710</v>
+        <v>44713</v>
       </c>
       <c r="AN7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44711</v>
+        <v>44714</v>
       </c>
       <c r="AO7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44712</v>
+        <v>44715</v>
       </c>
       <c r="AP7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44713</v>
+        <v>44716</v>
       </c>
       <c r="AQ7" s="62">
         <f ca="1">AP7+1</f>
-        <v>44714</v>
+        <v>44717</v>
       </c>
       <c r="AR7" s="62">
         <f ca="1">AQ7+1</f>
-        <v>44715</v>
+        <v>44718</v>
       </c>
       <c r="AS7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44716</v>
+        <v>44719</v>
       </c>
       <c r="AT7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="AU7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44718</v>
+        <v>44721</v>
       </c>
       <c r="AV7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44719</v>
+        <v>44722</v>
       </c>
       <c r="AW7" s="62">
         <f t="shared" ca="1" si="0"/>
-        <v>44720</v>
+        <v>44723</v>
       </c>
       <c r="AX7" s="62">
         <f ca="1">AW7+1</f>
-        <v>44721</v>
+        <v>44724</v>
       </c>
       <c r="AY7" s="62">
         <f ca="1">AX7+1</f>
-        <v>44722</v>
+        <v>44725</v>
       </c>
       <c r="AZ7" s="62">
         <f t="shared" ref="AZ7:BD7" ca="1" si="1">AY7+1</f>
-        <v>44723</v>
+        <v>44726</v>
       </c>
       <c r="BA7" s="62">
         <f t="shared" ca="1" si="1"/>
-        <v>44724</v>
+        <v>44727</v>
       </c>
       <c r="BB7" s="62">
         <f t="shared" ca="1" si="1"/>
-        <v>44725</v>
+        <v>44728</v>
       </c>
       <c r="BC7" s="62">
         <f t="shared" ca="1" si="1"/>
-        <v>44726</v>
+        <v>44729</v>
       </c>
       <c r="BD7" s="62">
         <f t="shared" ca="1" si="1"/>
-        <v>44727</v>
+        <v>44730</v>
       </c>
       <c r="BE7" s="62">
         <f ca="1">BD7+1</f>
-        <v>44728</v>
+        <v>44731</v>
       </c>
       <c r="BF7" s="62">
         <f ca="1">BE7+1</f>
-        <v>44729</v>
+        <v>44732</v>
       </c>
       <c r="BG7" s="62">
         <f t="shared" ref="BG7:BK7" ca="1" si="2">BF7+1</f>
-        <v>44730</v>
+        <v>44733</v>
       </c>
       <c r="BH7" s="62">
         <f t="shared" ca="1" si="2"/>
-        <v>44731</v>
+        <v>44734</v>
       </c>
       <c r="BI7" s="62">
         <f t="shared" ca="1" si="2"/>
-        <v>44732</v>
+        <v>44735</v>
       </c>
       <c r="BJ7" s="62">
         <f t="shared" ca="1" si="2"/>
-        <v>44733</v>
+        <v>44736</v>
       </c>
       <c r="BK7" s="77">
         <f t="shared" ca="1" si="2"/>
-        <v>44734</v>
+        <v>44737</v>
       </c>
     </row>
     <row r="8" spans="1:63" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -7242,7 +7242,7 @@
       <c r="G8" s="79"/>
       <c r="H8" s="63" t="str">
         <f ca="1">LEFT(TEXT(H7,"ddd"),1)</f>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="I8" s="60" t="str">
         <f ca="1">LEFT(TEXT(I7,"ddd"),1)</f>
@@ -7250,27 +7250,27 @@
       </c>
       <c r="J8" s="60" t="str">
         <f ca="1">LEFT(TEXT(J7,"ddd"),1)</f>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="K8" s="60" t="str">
         <f t="shared" ref="K8:BK8" ca="1" si="3">LEFT(TEXT(K7,"ddd"),1)</f>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="L8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="M8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="N8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="O8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="P8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7278,27 +7278,27 @@
       </c>
       <c r="Q8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="R8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="S8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="T8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="U8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="V8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="W8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7306,27 +7306,27 @@
       </c>
       <c r="X8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="Y8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="Z8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AA8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AB8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AC8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="AD8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7334,27 +7334,27 @@
       </c>
       <c r="AE8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="AF8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="AG8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AH8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AI8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AJ8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="AK8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7362,27 +7362,27 @@
       </c>
       <c r="AL8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="AM8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="AN8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AO8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AP8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AQ8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="AR8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7390,27 +7390,27 @@
       </c>
       <c r="AS8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="AT8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="AU8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AV8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AW8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AX8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="AY8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7418,27 +7418,27 @@
       </c>
       <c r="AZ8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="BA8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="BB8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="BC8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="BD8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="BE8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="BF8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -7446,23 +7446,23 @@
       </c>
       <c r="BG8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="BH8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="BI8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="BJ8" s="60" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="BK8" s="78" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
     </row>
     <row r="9" spans="1:63" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7774,7 +7774,7 @@
       </c>
       <c r="E11" s="51">
         <f ca="1">TODAY()</f>
-        <v>44669</v>
+        <v>44672</v>
       </c>
       <c r="F11" s="49">
         <v>3</v>
@@ -8014,7 +8014,7 @@
       <c r="D12" s="53"/>
       <c r="E12" s="51">
         <f ca="1">TODAY()+5</f>
-        <v>44674</v>
+        <v>44677</v>
       </c>
       <c r="F12" s="49">
         <v>1</v>
@@ -8256,7 +8256,7 @@
       </c>
       <c r="E13" s="51">
         <f ca="1">TODAY()-3</f>
-        <v>44666</v>
+        <v>44669</v>
       </c>
       <c r="F13" s="49">
         <v>10</v>
@@ -8496,7 +8496,7 @@
       <c r="D14" s="53"/>
       <c r="E14" s="51">
         <f ca="1">TODAY()+20</f>
-        <v>44689</v>
+        <v>44692</v>
       </c>
       <c r="F14" s="49">
         <v>1</v>
@@ -8738,7 +8738,7 @@
       </c>
       <c r="E15" s="51">
         <f ca="1">TODAY()+6</f>
-        <v>44675</v>
+        <v>44678</v>
       </c>
       <c r="F15" s="49">
         <v>6</v>
@@ -9215,7 +9215,7 @@
       </c>
       <c r="E17" s="51">
         <f ca="1">TODAY()+6</f>
-        <v>44675</v>
+        <v>44678</v>
       </c>
       <c r="F17" s="49">
         <v>13</v>
@@ -9457,7 +9457,7 @@
       </c>
       <c r="E18" s="51">
         <f ca="1">TODAY()+7</f>
-        <v>44676</v>
+        <v>44679</v>
       </c>
       <c r="F18" s="49">
         <v>9</v>
@@ -9699,7 +9699,7 @@
       </c>
       <c r="E19" s="51">
         <f ca="1">TODAY()+15</f>
-        <v>44684</v>
+        <v>44687</v>
       </c>
       <c r="F19" s="49">
         <v>11</v>
@@ -9939,7 +9939,7 @@
       <c r="D20" s="53"/>
       <c r="E20" s="51">
         <f ca="1">TODAY()+24</f>
-        <v>44693</v>
+        <v>44696</v>
       </c>
       <c r="F20" s="49">
         <v>1</v>
@@ -10179,7 +10179,7 @@
       <c r="D21" s="104"/>
       <c r="E21" s="51">
         <f ca="1">TODAY()+25</f>
-        <v>44694</v>
+        <v>44697</v>
       </c>
       <c r="F21" s="49">
         <v>24</v>
@@ -10654,7 +10654,7 @@
       <c r="D23" s="104"/>
       <c r="E23" s="51">
         <f ca="1">TODAY()+15</f>
-        <v>44684</v>
+        <v>44687</v>
       </c>
       <c r="F23" s="49">
         <v>4</v>
@@ -10894,7 +10894,7 @@
       <c r="D24" s="53"/>
       <c r="E24" s="51">
         <f ca="1">TODAY()+19</f>
-        <v>44688</v>
+        <v>44691</v>
       </c>
       <c r="F24" s="49">
         <v>14</v>
@@ -11134,7 +11134,7 @@
       <c r="D25" s="104"/>
       <c r="E25" s="51">
         <f ca="1">TODAY()+35</f>
-        <v>44704</v>
+        <v>44707</v>
       </c>
       <c r="F25" s="49">
         <v>6</v>
@@ -11374,7 +11374,7 @@
       <c r="D26" s="53"/>
       <c r="E26" s="51">
         <f ca="1">TODAY()+48</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="F26" s="49">
         <v>3</v>
@@ -11614,7 +11614,7 @@
       <c r="D27" s="104"/>
       <c r="E27" s="51">
         <f ca="1">TODAY()+40</f>
-        <v>44709</v>
+        <v>44712</v>
       </c>
       <c r="F27" s="49">
         <v>19</v>
@@ -12089,7 +12089,7 @@
       <c r="D29" s="104"/>
       <c r="E29" s="51">
         <f ca="1">TODAY()+37</f>
-        <v>44706</v>
+        <v>44709</v>
       </c>
       <c r="F29" s="49">
         <v>15</v>
@@ -12329,7 +12329,7 @@
       <c r="D30" s="53"/>
       <c r="E30" s="51">
         <f ca="1">TODAY()+29</f>
-        <v>44698</v>
+        <v>44701</v>
       </c>
       <c r="F30" s="49">
         <v>5</v>
@@ -12569,7 +12569,7 @@
       <c r="D31" s="104"/>
       <c r="E31" s="51">
         <f ca="1">TODAY()+80</f>
-        <v>44749</v>
+        <v>44752</v>
       </c>
       <c r="F31" s="49">
         <v>5</v>
@@ -13958,7 +13958,7 @@
       </c>
       <c r="C5" s="56">
         <f ca="1">IFERROR(IF(MIN(Milestones[Start])=0,TODAY(),MIN(Milestones[Start])),TODAY())</f>
-        <v>44666</v>
+        <v>44669</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="73"/>
@@ -14041,7 +14041,7 @@
       <c r="G6" s="12"/>
       <c r="H6" s="89" t="str">
         <f ca="1">TEXT(H7,"mmmm")</f>
-        <v>abril</v>
+        <v>maio</v>
       </c>
       <c r="I6" s="89"/>
       <c r="J6" s="89"/>
@@ -14051,7 +14051,7 @@
       <c r="N6" s="29"/>
       <c r="O6" s="29" t="str">
         <f ca="1">IF(TEXT(O7,"mmmm")=H6,"",TEXT(O7,"mmmm"))</f>
-        <v>maio</v>
+        <v/>
       </c>
       <c r="P6" s="29"/>
       <c r="Q6" s="29"/>
@@ -14129,227 +14129,227 @@
       <c r="G7" s="23"/>
       <c r="H7" s="64">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>44679</v>
+        <v>44682</v>
       </c>
       <c r="I7" s="66">
         <f ca="1">H7+1</f>
-        <v>44680</v>
+        <v>44683</v>
       </c>
       <c r="J7" s="66">
         <f t="shared" ref="J7:AW7" ca="1" si="0">I7+1</f>
-        <v>44681</v>
+        <v>44684</v>
       </c>
       <c r="K7" s="66">
         <f ca="1">J7+1</f>
-        <v>44682</v>
+        <v>44685</v>
       </c>
       <c r="L7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44683</v>
+        <v>44686</v>
       </c>
       <c r="M7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44684</v>
+        <v>44687</v>
       </c>
       <c r="N7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44685</v>
+        <v>44688</v>
       </c>
       <c r="O7" s="66">
         <f ca="1">N7+1</f>
-        <v>44686</v>
+        <v>44689</v>
       </c>
       <c r="P7" s="66">
         <f ca="1">O7+1</f>
-        <v>44687</v>
+        <v>44690</v>
       </c>
       <c r="Q7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44688</v>
+        <v>44691</v>
       </c>
       <c r="R7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44689</v>
+        <v>44692</v>
       </c>
       <c r="S7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44690</v>
+        <v>44693</v>
       </c>
       <c r="T7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44691</v>
+        <v>44694</v>
       </c>
       <c r="U7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44692</v>
+        <v>44695</v>
       </c>
       <c r="V7" s="66">
         <f ca="1">U7+1</f>
-        <v>44693</v>
+        <v>44696</v>
       </c>
       <c r="W7" s="66">
         <f ca="1">V7+1</f>
-        <v>44694</v>
+        <v>44697</v>
       </c>
       <c r="X7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44695</v>
+        <v>44698</v>
       </c>
       <c r="Y7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44696</v>
+        <v>44699</v>
       </c>
       <c r="Z7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44697</v>
+        <v>44700</v>
       </c>
       <c r="AA7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44698</v>
+        <v>44701</v>
       </c>
       <c r="AB7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44699</v>
+        <v>44702</v>
       </c>
       <c r="AC7" s="66">
         <f ca="1">AB7+1</f>
-        <v>44700</v>
+        <v>44703</v>
       </c>
       <c r="AD7" s="66">
         <f ca="1">AC7+1</f>
-        <v>44701</v>
+        <v>44704</v>
       </c>
       <c r="AE7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44702</v>
+        <v>44705</v>
       </c>
       <c r="AF7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44703</v>
+        <v>44706</v>
       </c>
       <c r="AG7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44704</v>
+        <v>44707</v>
       </c>
       <c r="AH7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44705</v>
+        <v>44708</v>
       </c>
       <c r="AI7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44706</v>
+        <v>44709</v>
       </c>
       <c r="AJ7" s="66">
         <f ca="1">AI7+1</f>
-        <v>44707</v>
+        <v>44710</v>
       </c>
       <c r="AK7" s="66">
         <f ca="1">AJ7+1</f>
-        <v>44708</v>
+        <v>44711</v>
       </c>
       <c r="AL7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44709</v>
+        <v>44712</v>
       </c>
       <c r="AM7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44710</v>
+        <v>44713</v>
       </c>
       <c r="AN7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44711</v>
+        <v>44714</v>
       </c>
       <c r="AO7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44712</v>
+        <v>44715</v>
       </c>
       <c r="AP7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44713</v>
+        <v>44716</v>
       </c>
       <c r="AQ7" s="66">
         <f ca="1">AP7+1</f>
-        <v>44714</v>
+        <v>44717</v>
       </c>
       <c r="AR7" s="66">
         <f ca="1">AQ7+1</f>
-        <v>44715</v>
+        <v>44718</v>
       </c>
       <c r="AS7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44716</v>
+        <v>44719</v>
       </c>
       <c r="AT7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="AU7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44718</v>
+        <v>44721</v>
       </c>
       <c r="AV7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44719</v>
+        <v>44722</v>
       </c>
       <c r="AW7" s="66">
         <f t="shared" ca="1" si="0"/>
-        <v>44720</v>
+        <v>44723</v>
       </c>
       <c r="AX7" s="66">
         <f ca="1">AW7+1</f>
-        <v>44721</v>
+        <v>44724</v>
       </c>
       <c r="AY7" s="66">
         <f ca="1">AX7+1</f>
-        <v>44722</v>
+        <v>44725</v>
       </c>
       <c r="AZ7" s="66">
         <f t="shared" ref="AZ7:BD7" ca="1" si="1">AY7+1</f>
-        <v>44723</v>
+        <v>44726</v>
       </c>
       <c r="BA7" s="66">
         <f t="shared" ca="1" si="1"/>
-        <v>44724</v>
+        <v>44727</v>
       </c>
       <c r="BB7" s="66">
         <f t="shared" ca="1" si="1"/>
-        <v>44725</v>
+        <v>44728</v>
       </c>
       <c r="BC7" s="66">
         <f t="shared" ca="1" si="1"/>
-        <v>44726</v>
+        <v>44729</v>
       </c>
       <c r="BD7" s="66">
         <f t="shared" ca="1" si="1"/>
-        <v>44727</v>
+        <v>44730</v>
       </c>
       <c r="BE7" s="66">
         <f ca="1">BD7+1</f>
-        <v>44728</v>
+        <v>44731</v>
       </c>
       <c r="BF7" s="66">
         <f ca="1">BE7+1</f>
-        <v>44729</v>
+        <v>44732</v>
       </c>
       <c r="BG7" s="66">
         <f t="shared" ref="BG7:BK7" ca="1" si="2">BF7+1</f>
-        <v>44730</v>
+        <v>44733</v>
       </c>
       <c r="BH7" s="66">
         <f t="shared" ca="1" si="2"/>
-        <v>44731</v>
+        <v>44734</v>
       </c>
       <c r="BI7" s="66">
         <f t="shared" ca="1" si="2"/>
-        <v>44732</v>
+        <v>44735</v>
       </c>
       <c r="BJ7" s="66">
         <f t="shared" ca="1" si="2"/>
-        <v>44733</v>
+        <v>44736</v>
       </c>
       <c r="BK7" s="30">
         <f t="shared" ca="1" si="2"/>
-        <v>44734</v>
+        <v>44737</v>
       </c>
     </row>
     <row r="8" spans="1:63" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -14372,7 +14372,7 @@
       <c r="G8" s="69"/>
       <c r="H8" s="68" t="str">
         <f ca="1">LEFT(TEXT(H7,"ddd"),1)</f>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="I8" s="67" t="str">
         <f ca="1">LEFT(TEXT(I7,"ddd"),1)</f>
@@ -14380,27 +14380,27 @@
       </c>
       <c r="J8" s="67" t="str">
         <f ca="1">LEFT(TEXT(J7,"ddd"),1)</f>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="K8" s="67" t="str">
         <f t="shared" ref="K8:AM8" ca="1" si="3">LEFT(TEXT(K7,"ddd"),1)</f>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="L8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="M8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="N8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="O8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="P8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -14408,27 +14408,27 @@
       </c>
       <c r="Q8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="R8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="S8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="T8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="U8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="V8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="W8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -14436,27 +14436,27 @@
       </c>
       <c r="X8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="Y8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="Z8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AA8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AB8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AC8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="AD8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -14464,27 +14464,27 @@
       </c>
       <c r="AE8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="AF8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="AG8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AH8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AI8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AJ8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="AK8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -14492,27 +14492,27 @@
       </c>
       <c r="AL8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="AM8" s="67" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="AN8" s="67" t="str">
         <f t="shared" ref="AN8:BK8" ca="1" si="4">LEFT(TEXT(AN7,"ddd"),1)</f>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AO8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AP8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AQ8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="AR8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -14520,27 +14520,27 @@
       </c>
       <c r="AS8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="AT8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="AU8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="AV8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="AW8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="AX8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="AY8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -14548,27 +14548,27 @@
       </c>
       <c r="AZ8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="BA8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="BB8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="BC8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="BD8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>q</v>
+        <v>s</v>
       </c>
       <c r="BE8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>q</v>
+        <v>d</v>
       </c>
       <c r="BF8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -14576,23 +14576,23 @@
       </c>
       <c r="BG8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>t</v>
       </c>
       <c r="BH8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>q</v>
       </c>
       <c r="BI8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>q</v>
       </c>
       <c r="BJ8" s="67" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>t</v>
+        <v>s</v>
       </c>
       <c r="BK8" s="65" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>q</v>
+        <v>s</v>
       </c>
     </row>
     <row r="9" spans="1:63" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -14905,7 +14905,7 @@
       </c>
       <c r="E11" s="51">
         <f ca="1">TODAY()</f>
-        <v>44669</v>
+        <v>44672</v>
       </c>
       <c r="F11" s="49">
         <v>3</v>
@@ -15145,7 +15145,7 @@
       <c r="D12" s="52"/>
       <c r="E12" s="51">
         <f ca="1">TODAY()+5</f>
-        <v>44674</v>
+        <v>44677</v>
       </c>
       <c r="F12" s="49">
         <v>1</v>
@@ -15387,7 +15387,7 @@
       </c>
       <c r="E13" s="51">
         <f ca="1">TODAY()-3</f>
-        <v>44666</v>
+        <v>44669</v>
       </c>
       <c r="F13" s="49">
         <v>10</v>
@@ -15627,7 +15627,7 @@
       <c r="D14" s="52"/>
       <c r="E14" s="51">
         <f ca="1">TODAY()+20</f>
-        <v>44689</v>
+        <v>44692</v>
       </c>
       <c r="F14" s="49">
         <v>1</v>
@@ -15869,7 +15869,7 @@
       </c>
       <c r="E15" s="51">
         <f ca="1">TODAY()+6</f>
-        <v>44675</v>
+        <v>44678</v>
       </c>
       <c r="F15" s="49">
         <v>6</v>
@@ -16346,7 +16346,7 @@
       </c>
       <c r="E17" s="51">
         <f ca="1">TODAY()+6</f>
-        <v>44675</v>
+        <v>44678</v>
       </c>
       <c r="F17" s="49">
         <v>13</v>
@@ -16588,7 +16588,7 @@
       </c>
       <c r="E18" s="51">
         <f ca="1">TODAY()+7</f>
-        <v>44676</v>
+        <v>44679</v>
       </c>
       <c r="F18" s="49">
         <v>9</v>
@@ -16830,7 +16830,7 @@
       </c>
       <c r="E19" s="51">
         <f ca="1">TODAY()+15</f>
-        <v>44684</v>
+        <v>44687</v>
       </c>
       <c r="F19" s="49">
         <v>11</v>
@@ -17070,7 +17070,7 @@
       <c r="D20" s="52"/>
       <c r="E20" s="51">
         <f ca="1">TODAY()+24</f>
-        <v>44693</v>
+        <v>44696</v>
       </c>
       <c r="F20" s="49">
         <v>1</v>
@@ -17310,7 +17310,7 @@
       <c r="D21" s="52"/>
       <c r="E21" s="51">
         <f ca="1">TODAY()+25</f>
-        <v>44694</v>
+        <v>44697</v>
       </c>
       <c r="F21" s="49">
         <v>24</v>
@@ -17785,7 +17785,7 @@
       <c r="D23" s="52"/>
       <c r="E23" s="51">
         <f ca="1">TODAY()+15</f>
-        <v>44684</v>
+        <v>44687</v>
       </c>
       <c r="F23" s="49">
         <v>4</v>
@@ -18025,7 +18025,7 @@
       <c r="D24" s="52"/>
       <c r="E24" s="51">
         <f ca="1">TODAY()+19</f>
-        <v>44688</v>
+        <v>44691</v>
       </c>
       <c r="F24" s="49">
         <v>14</v>
@@ -18265,7 +18265,7 @@
       <c r="D25" s="52"/>
       <c r="E25" s="51">
         <f ca="1">TODAY()+35</f>
-        <v>44704</v>
+        <v>44707</v>
       </c>
       <c r="F25" s="49">
         <v>6</v>
@@ -18505,7 +18505,7 @@
       <c r="D26" s="52"/>
       <c r="E26" s="51">
         <f ca="1">TODAY()+48</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="F26" s="49">
         <v>3</v>
@@ -18745,7 +18745,7 @@
       <c r="D27" s="52"/>
       <c r="E27" s="51">
         <f ca="1">TODAY()+40</f>
-        <v>44709</v>
+        <v>44712</v>
       </c>
       <c r="F27" s="49">
         <v>19</v>
@@ -19220,7 +19220,7 @@
       <c r="D29" s="52"/>
       <c r="E29" s="51">
         <f ca="1">TODAY()+37</f>
-        <v>44706</v>
+        <v>44709</v>
       </c>
       <c r="F29" s="49">
         <v>15</v>
@@ -19460,7 +19460,7 @@
       <c r="D30" s="52"/>
       <c r="E30" s="51">
         <f ca="1">TODAY()+29</f>
-        <v>44698</v>
+        <v>44701</v>
       </c>
       <c r="F30" s="49">
         <v>5</v>
@@ -19700,7 +19700,7 @@
       <c r="D31" s="52"/>
       <c r="E31" s="51">
         <f ca="1">TODAY()+80</f>
-        <v>44749</v>
+        <v>44752</v>
       </c>
       <c r="F31" s="49">
         <v>5</v>

</xml_diff>